<commit_message>
ggplot de excel, entidades particitpantes 1
</commit_message>
<xml_diff>
--- a/datos/SIPAP_pestañas/Entidades Financieras 01.xlsx
+++ b/datos/SIPAP_pestañas/Entidades Financieras 01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrabajoPracticoR\RStudio\datos\SIPAP_pestañas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\RStudio\RStudio\datos\SIPAP_pestañas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{622D4F66-AE21-4913-84A4-FCA5B20F6E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8629F6-456D-4B79-AA6D-BAE1135108FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{06599D00-516B-411A-B56B-0FC5F4E86451}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{06599D00-516B-411A-B56B-0FC5F4E86451}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +425,13 @@
       <sz val="10"/>
       <name val="BaskervilleTMed"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -468,10 +478,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -491,8 +502,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -808,16 +827,16 @@
   <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.47265625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="41.4">
+    <row r="1" spans="1:7" ht="42.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -830,7 +849,7 @@
       <c r="D1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -853,7 +872,7 @@
       <c r="D2" s="4">
         <v>716</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="8">
         <v>365625582883</v>
       </c>
       <c r="F2" s="4">
@@ -876,7 +895,7 @@
       <c r="D3" s="4">
         <v>3796</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="8">
         <v>2672801044341</v>
       </c>
       <c r="F3" s="4">
@@ -899,7 +918,7 @@
       <c r="D4" s="4">
         <v>4194</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <v>2076399423174</v>
       </c>
       <c r="F4" s="4">
@@ -918,7 +937,7 @@
       <c r="D5" s="4">
         <v>4140</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="8">
         <v>2230991173706</v>
       </c>
       <c r="F5" s="4">
@@ -937,7 +956,7 @@
       <c r="D6" s="4">
         <v>4511</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="8">
         <v>2588383672152</v>
       </c>
       <c r="F6" s="4">
@@ -956,7 +975,7 @@
       <c r="D7" s="4">
         <v>4214</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="8">
         <v>2623533732696</v>
       </c>
       <c r="F7" s="4">
@@ -975,7 +994,7 @@
       <c r="D8" s="4">
         <v>4151</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="8">
         <v>2520176027668</v>
       </c>
       <c r="F8" s="4">
@@ -994,7 +1013,7 @@
       <c r="D9" s="4">
         <v>4356</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="8">
         <v>2452198704854</v>
       </c>
       <c r="F9" s="4">
@@ -1013,7 +1032,7 @@
       <c r="D10" s="4">
         <v>5118</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="8">
         <v>2771320301354</v>
       </c>
       <c r="F10" s="4">
@@ -1032,7 +1051,7 @@
       <c r="D11" s="4">
         <v>4712</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="8">
         <v>2434690908734</v>
       </c>
       <c r="F11" s="4">
@@ -1051,7 +1070,7 @@
       <c r="D12" s="4">
         <v>5197</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="8">
         <v>3323952356600</v>
       </c>
       <c r="F12" s="4">
@@ -1070,7 +1089,7 @@
       <c r="D13" s="4">
         <v>5549</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="8">
         <v>4082554385623</v>
       </c>
       <c r="F13" s="4">
@@ -1089,7 +1108,7 @@
       <c r="D14" s="4">
         <v>2458</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="8">
         <v>2967118404654</v>
       </c>
       <c r="F14" s="4">
@@ -1108,7 +1127,7 @@
       <c r="D15" s="4">
         <v>2692</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="8">
         <v>3067729582116</v>
       </c>
       <c r="F15" s="4">
@@ -1127,7 +1146,7 @@
       <c r="D16" s="4">
         <v>2639</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="8">
         <v>2544131871210</v>
       </c>
       <c r="F16" s="4">
@@ -1146,7 +1165,7 @@
       <c r="D17" s="4">
         <v>2449</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="8">
         <v>2518726386279</v>
       </c>
       <c r="F17" s="4">
@@ -1165,7 +1184,7 @@
       <c r="D18" s="4">
         <v>3013</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="8">
         <v>3230054956091</v>
       </c>
       <c r="F18" s="4">
@@ -1184,7 +1203,7 @@
       <c r="D19" s="4">
         <v>2607</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="8">
         <v>2921499644045</v>
       </c>
       <c r="F19" s="4">
@@ -1203,7 +1222,7 @@
       <c r="D20" s="4">
         <v>2314</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="8">
         <v>2548564778894</v>
       </c>
       <c r="F20" s="4">
@@ -1222,7 +1241,7 @@
       <c r="D21" s="4">
         <v>2494</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="8">
         <v>2688158941779</v>
       </c>
       <c r="F21" s="4">
@@ -1245,7 +1264,7 @@
       <c r="D22" s="4">
         <v>2736</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="8">
         <v>2752663244304</v>
       </c>
       <c r="F22" s="4">
@@ -1264,7 +1283,7 @@
       <c r="D23" s="4">
         <v>2507</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="8">
         <v>2559342060372</v>
       </c>
       <c r="F23" s="4">
@@ -1283,7 +1302,7 @@
       <c r="D24" s="4">
         <v>2311</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="8">
         <v>2395380793881</v>
       </c>
       <c r="F24" s="4">
@@ -1302,7 +1321,7 @@
       <c r="D25" s="4">
         <v>2975</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="8">
         <v>3368634902247</v>
       </c>
       <c r="F25" s="4">
@@ -1321,7 +1340,7 @@
       <c r="D26" s="4">
         <v>2803</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="8">
         <v>2925812367635</v>
       </c>
       <c r="F26" s="4">
@@ -1344,7 +1363,7 @@
       <c r="D27" s="4">
         <v>2632</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="8">
         <v>2643166643943</v>
       </c>
       <c r="F27" s="4">
@@ -1367,7 +1386,7 @@
       <c r="D28" s="4">
         <v>2207</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="8">
         <v>2357101300498</v>
       </c>
       <c r="F28" s="4">
@@ -1386,7 +1405,7 @@
       <c r="D29" s="4">
         <v>2680</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="8">
         <v>3108624283530</v>
       </c>
       <c r="F29" s="4">
@@ -1405,7 +1424,7 @@
       <c r="D30" s="4">
         <v>3305</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="8">
         <v>4061564810922</v>
       </c>
       <c r="F30" s="4">
@@ -1424,7 +1443,7 @@
       <c r="D31" s="4">
         <v>3034</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="8">
         <v>3472871768706</v>
       </c>
       <c r="F31" s="4">
@@ -1443,7 +1462,7 @@
       <c r="D32" s="4">
         <v>3237</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="8">
         <v>4161482325086</v>
       </c>
       <c r="F32" s="4">
@@ -1462,7 +1481,7 @@
       <c r="D33" s="4">
         <v>3117</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="8">
         <v>4014344326213</v>
       </c>
       <c r="F33" s="4">
@@ -1481,7 +1500,7 @@
       <c r="D34" s="4">
         <v>3208</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="8">
         <v>3848779294556</v>
       </c>
       <c r="F34" s="4">
@@ -1500,7 +1519,7 @@
       <c r="D35" s="4">
         <v>3321</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="8">
         <v>4019435332052</v>
       </c>
       <c r="F35" s="4">
@@ -1519,7 +1538,7 @@
       <c r="D36" s="4">
         <v>3215</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="8">
         <v>3932463818099</v>
       </c>
       <c r="F36" s="4">
@@ -1538,7 +1557,7 @@
       <c r="D37" s="4">
         <v>3046</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="8">
         <v>3561602654228</v>
       </c>
       <c r="F37" s="4">
@@ -1557,7 +1576,7 @@
       <c r="D38" s="4">
         <v>2880</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="8">
         <v>3459727554753</v>
       </c>
       <c r="F38" s="4">
@@ -1580,7 +1599,7 @@
       <c r="D39" s="4">
         <v>3265</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="8">
         <v>3877577181206</v>
       </c>
       <c r="F39" s="4">
@@ -1599,7 +1618,7 @@
       <c r="D40" s="4">
         <v>2969</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="8">
         <v>3948236563867</v>
       </c>
       <c r="F40" s="4">
@@ -1622,7 +1641,7 @@
       <c r="D41" s="4">
         <v>2953</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="8">
         <v>3917472663021</v>
       </c>
       <c r="F41" s="4">
@@ -1641,7 +1660,7 @@
       <c r="D42" s="4">
         <v>3910</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="8">
         <v>4823545893470</v>
       </c>
       <c r="F42" s="4">
@@ -1660,7 +1679,7 @@
       <c r="D43" s="4">
         <v>2966</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="8">
         <v>3602946021320</v>
       </c>
       <c r="F43" s="4">
@@ -1679,7 +1698,7 @@
       <c r="D44" s="4">
         <v>3259</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="8">
         <v>3994844797791</v>
       </c>
       <c r="F44" s="4">
@@ -1702,7 +1721,7 @@
       <c r="D45" s="4">
         <v>3117</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="8">
         <v>3888997143948</v>
       </c>
       <c r="F45" s="4">
@@ -1721,7 +1740,7 @@
       <c r="D46" s="4">
         <v>3269</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="8">
         <v>3834592304603</v>
       </c>
       <c r="F46" s="4">
@@ -1744,7 +1763,7 @@
       <c r="D47" s="4">
         <v>3285</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="8">
         <v>3825789361069</v>
       </c>
       <c r="F47" s="4">
@@ -1763,7 +1782,7 @@
       <c r="D48" s="4">
         <v>3196</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="8">
         <v>3963245278170</v>
       </c>
       <c r="F48" s="4">
@@ -1786,7 +1805,7 @@
       <c r="D49" s="4">
         <v>3182</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="8">
         <v>3866852299654</v>
       </c>
       <c r="F49" s="4">
@@ -1805,7 +1824,7 @@
       <c r="D50" s="4">
         <v>3086</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="8">
         <v>3888873083607</v>
       </c>
       <c r="F50" s="4">
@@ -1828,7 +1847,7 @@
       <c r="D51" s="4">
         <v>3492</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="8">
         <v>4428764219543</v>
       </c>
       <c r="F51" s="4">
@@ -1847,7 +1866,7 @@
       <c r="D52" s="4">
         <v>3203</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="8">
         <v>3924956073761</v>
       </c>
       <c r="F52" s="4">
@@ -1866,7 +1885,7 @@
       <c r="D53" s="4">
         <v>2760</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="8">
         <v>3713773367227</v>
       </c>
       <c r="F53" s="4">
@@ -1889,7 +1908,7 @@
       <c r="D54" s="4">
         <v>3184</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="8">
         <v>4320243826364</v>
       </c>
       <c r="F54" s="4">
@@ -1908,7 +1927,7 @@
       <c r="D55" s="4">
         <v>2903</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="8">
         <v>4605704771499</v>
       </c>
       <c r="F55" s="4">
@@ -1931,7 +1950,7 @@
       <c r="D56" s="4">
         <v>3116</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="8">
         <v>4616494971060</v>
       </c>
       <c r="F56" s="4">
@@ -1954,7 +1973,7 @@
       <c r="D57" s="4">
         <v>2873</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="8">
         <v>4527592504933</v>
       </c>
       <c r="F57" s="4">
@@ -1973,7 +1992,7 @@
       <c r="D58" s="4">
         <v>2734</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="8">
         <v>4659709184198</v>
       </c>
       <c r="F58" s="4">
@@ -1992,7 +2011,7 @@
       <c r="D59" s="4">
         <v>2793</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="8">
         <v>4830708403321</v>
       </c>
       <c r="F59" s="4">
@@ -2011,7 +2030,7 @@
       <c r="D60" s="4">
         <v>2634</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E60" s="8">
         <v>4562643309337</v>
       </c>
       <c r="F60" s="4">
@@ -2030,7 +2049,7 @@
       <c r="D61" s="4">
         <v>2825</v>
       </c>
-      <c r="E61" s="4">
+      <c r="E61" s="8">
         <v>4851758056795</v>
       </c>
       <c r="F61" s="4">
@@ -2049,7 +2068,7 @@
       <c r="D62" s="4">
         <v>3204</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="8">
         <v>5455440471619</v>
       </c>
       <c r="F62" s="4">
@@ -2072,7 +2091,7 @@
       <c r="D63" s="4">
         <v>2961</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="8">
         <v>5422827445944</v>
       </c>
       <c r="F63" s="4">
@@ -2091,7 +2110,7 @@
       <c r="D64" s="4">
         <v>3283</v>
       </c>
-      <c r="E64" s="4">
+      <c r="E64" s="8">
         <v>5934063066576</v>
       </c>
       <c r="F64" s="4">
@@ -2114,7 +2133,7 @@
       <c r="D65" s="4">
         <v>3101</v>
       </c>
-      <c r="E65" s="4">
+      <c r="E65" s="8">
         <v>5309134598755</v>
       </c>
       <c r="F65" s="4">
@@ -2133,7 +2152,7 @@
       <c r="D66" s="4">
         <v>2982</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="8">
         <v>5433693756752</v>
       </c>
       <c r="F66" s="4">
@@ -2152,7 +2171,7 @@
       <c r="D67" s="4">
         <v>2745</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67" s="8">
         <v>5286484855404</v>
       </c>
       <c r="F67" s="4">
@@ -2171,7 +2190,7 @@
       <c r="D68" s="4">
         <v>3000</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="8">
         <v>6139800352549</v>
       </c>
       <c r="F68" s="4">
@@ -2190,7 +2209,7 @@
       <c r="D69" s="4">
         <v>2812</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="8">
         <v>5466270836609</v>
       </c>
       <c r="F69" s="4">
@@ -2209,7 +2228,7 @@
       <c r="D70" s="4">
         <v>3400</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E70" s="8">
         <v>6480469852505</v>
       </c>
       <c r="F70" s="4">
@@ -2228,7 +2247,7 @@
       <c r="D71" s="4">
         <v>3494</v>
       </c>
-      <c r="E71" s="4">
+      <c r="E71" s="8">
         <v>6413641831626</v>
       </c>
       <c r="F71" s="4">
@@ -2247,7 +2266,7 @@
       <c r="D72" s="4">
         <v>3456</v>
       </c>
-      <c r="E72" s="4">
+      <c r="E72" s="8">
         <v>6864103835704</v>
       </c>
       <c r="F72" s="4">
@@ -2266,7 +2285,7 @@
       <c r="D73" s="4">
         <v>3438</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="8">
         <v>6539085607917</v>
       </c>
       <c r="F73" s="4">
@@ -2289,7 +2308,7 @@
       <c r="D74" s="4">
         <v>3041</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="8">
         <v>5754259045932</v>
       </c>
       <c r="F74" s="4">
@@ -2312,7 +2331,7 @@
       <c r="D75" s="4">
         <v>2916</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75" s="8">
         <v>5824450972123</v>
       </c>
       <c r="F75" s="4">
@@ -2335,7 +2354,7 @@
       <c r="D76" s="4">
         <v>2610</v>
       </c>
-      <c r="E76" s="4">
+      <c r="E76" s="8">
         <v>5139997767158</v>
       </c>
       <c r="F76" s="4">
@@ -2354,7 +2373,7 @@
       <c r="D77" s="4">
         <v>2875</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77" s="8">
         <v>5829879837072</v>
       </c>
       <c r="F77" s="4">
@@ -2373,7 +2392,7 @@
       <c r="D78" s="4">
         <v>3228</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78" s="8">
         <v>6627538521858</v>
       </c>
       <c r="F78" s="4">
@@ -2392,7 +2411,7 @@
       <c r="D79" s="4">
         <v>2489</v>
       </c>
-      <c r="E79" s="4">
+      <c r="E79" s="8">
         <v>5172451641493</v>
       </c>
       <c r="F79" s="4">
@@ -2415,7 +2434,7 @@
       <c r="D80" s="4">
         <v>2790</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80" s="8">
         <v>6017618112438</v>
       </c>
       <c r="F80" s="4">
@@ -2434,7 +2453,7 @@
       <c r="D81" s="4">
         <v>3284</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E81" s="8">
         <v>7178686331483</v>
       </c>
       <c r="F81" s="4">
@@ -2453,7 +2472,7 @@
       <c r="D82" s="4">
         <v>3530</v>
       </c>
-      <c r="E82" s="4">
+      <c r="E82" s="8">
         <v>7383533527604</v>
       </c>
       <c r="F82" s="4">
@@ -2472,7 +2491,7 @@
       <c r="D83" s="4">
         <v>3024</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="8">
         <v>6328418330018</v>
       </c>
       <c r="F83" s="4">
@@ -2491,7 +2510,7 @@
       <c r="D84" s="4">
         <v>2850</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="8">
         <v>6170449376003</v>
       </c>
       <c r="F84" s="4">
@@ -2514,7 +2533,7 @@
       <c r="D85" s="4">
         <v>3145</v>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="8">
         <v>6170758532789</v>
       </c>
       <c r="F85" s="4">
@@ -2533,7 +2552,7 @@
       <c r="D86" s="4">
         <v>2779</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86" s="8">
         <v>5506941881002</v>
       </c>
       <c r="F86" s="4">
@@ -2556,7 +2575,7 @@
       <c r="D87" s="4">
         <v>3097</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87" s="8">
         <v>6955260207831</v>
       </c>
       <c r="F87" s="4">
@@ -2575,7 +2594,7 @@
       <c r="D88" s="4">
         <v>2608</v>
       </c>
-      <c r="E88" s="4">
+      <c r="E88" s="8">
         <v>5168151026855</v>
       </c>
       <c r="F88" s="4">
@@ -2598,7 +2617,7 @@
       <c r="D89" s="4">
         <v>2542</v>
       </c>
-      <c r="E89" s="4">
+      <c r="E89" s="8">
         <v>5406060154606</v>
       </c>
       <c r="F89" s="4">
@@ -2621,7 +2640,7 @@
       <c r="D90" s="4">
         <v>3123</v>
       </c>
-      <c r="E90" s="4">
+      <c r="E90" s="8">
         <v>6095608956055</v>
       </c>
       <c r="F90" s="4">
@@ -2640,7 +2659,7 @@
       <c r="D91" s="4">
         <v>3002</v>
       </c>
-      <c r="E91" s="4">
+      <c r="E91" s="8">
         <v>5866609571342</v>
       </c>
       <c r="F91" s="4">
@@ -2659,7 +2678,7 @@
       <c r="D92" s="4">
         <v>3178</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E92" s="8">
         <v>6278603530203</v>
       </c>
       <c r="F92" s="4">
@@ -2682,7 +2701,7 @@
       <c r="D93" s="4">
         <v>3583</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E93" s="8">
         <v>7000628663346</v>
       </c>
       <c r="F93" s="4">
@@ -2701,7 +2720,7 @@
       <c r="D94" s="4">
         <v>3300</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E94" s="8">
         <v>6952633629717</v>
       </c>
       <c r="F94" s="4">
@@ -2720,7 +2739,7 @@
       <c r="D95" s="4">
         <v>3118</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E95" s="8">
         <v>6937280666089</v>
       </c>
       <c r="F95" s="4">
@@ -2739,7 +2758,7 @@
       <c r="D96" s="4">
         <v>3234</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E96" s="8">
         <v>6596263092008</v>
       </c>
       <c r="F96" s="4">
@@ -2758,7 +2777,7 @@
       <c r="D97" s="4">
         <v>3551</v>
       </c>
-      <c r="E97" s="4">
+      <c r="E97" s="8">
         <v>6927822288346</v>
       </c>
       <c r="F97" s="4">
@@ -2777,7 +2796,7 @@
       <c r="D98" s="4">
         <v>3537</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E98" s="8">
         <v>7372107183366</v>
       </c>
       <c r="F98" s="4">
@@ -2800,7 +2819,7 @@
       <c r="D99" s="4">
         <v>3951</v>
       </c>
-      <c r="E99" s="4">
+      <c r="E99" s="8">
         <v>8231432953541</v>
       </c>
       <c r="F99" s="4">
@@ -2823,7 +2842,7 @@
       <c r="D100" s="4">
         <v>2911</v>
       </c>
-      <c r="E100" s="4">
+      <c r="E100" s="8">
         <v>6406683314816</v>
       </c>
       <c r="F100" s="4">
@@ -2842,7 +2861,7 @@
       <c r="D101" s="4">
         <v>3017</v>
       </c>
-      <c r="E101" s="4">
+      <c r="E101" s="8">
         <v>6589658031721</v>
       </c>
       <c r="F101" s="4">
@@ -2861,7 +2880,7 @@
       <c r="D102" s="4">
         <v>3901</v>
       </c>
-      <c r="E102" s="4">
+      <c r="E102" s="8">
         <v>8424136250863</v>
       </c>
       <c r="F102" s="4">
@@ -2880,7 +2899,7 @@
       <c r="D103" s="4">
         <v>3269</v>
       </c>
-      <c r="E103" s="4">
+      <c r="E103" s="8">
         <v>6248683385351</v>
       </c>
       <c r="F103" s="4">
@@ -2899,7 +2918,7 @@
       <c r="D104" s="4">
         <v>3512</v>
       </c>
-      <c r="E104" s="4">
+      <c r="E104" s="8">
         <v>6734141992876</v>
       </c>
       <c r="F104" s="4">
@@ -2922,7 +2941,7 @@
       <c r="D105" s="4">
         <v>3562</v>
       </c>
-      <c r="E105" s="4">
+      <c r="E105" s="8">
         <v>7251874971778</v>
       </c>
       <c r="F105" s="4">
@@ -2941,7 +2960,7 @@
       <c r="D106" s="4">
         <v>3258</v>
       </c>
-      <c r="E106" s="4">
+      <c r="E106" s="8">
         <v>6421976353931</v>
       </c>
       <c r="F106" s="4">
@@ -2960,7 +2979,7 @@
       <c r="D107" s="4">
         <v>3938</v>
       </c>
-      <c r="E107" s="4">
+      <c r="E107" s="8">
         <v>12589827589514</v>
       </c>
       <c r="F107" s="4">
@@ -2979,7 +2998,7 @@
       <c r="D108" s="4">
         <v>4083</v>
       </c>
-      <c r="E108" s="4">
+      <c r="E108" s="8">
         <v>11008875716759</v>
       </c>
       <c r="F108" s="4">
@@ -3002,7 +3021,7 @@
       <c r="D109" s="4">
         <v>3704</v>
       </c>
-      <c r="E109" s="4">
+      <c r="E109" s="8">
         <v>9646818969036</v>
       </c>
       <c r="F109" s="4">
@@ -3025,7 +3044,7 @@
       <c r="D110" s="4">
         <v>3603</v>
       </c>
-      <c r="E110" s="4">
+      <c r="E110" s="8">
         <v>8998896215776</v>
       </c>
       <c r="F110" s="4">
@@ -3048,7 +3067,7 @@
       <c r="D111" s="4">
         <v>3422</v>
       </c>
-      <c r="E111" s="4">
+      <c r="E111" s="8">
         <v>9930422138933</v>
       </c>
       <c r="F111" s="4">
@@ -3067,7 +3086,7 @@
       <c r="D112" s="4">
         <v>3021</v>
       </c>
-      <c r="E112" s="4">
+      <c r="E112" s="8">
         <v>8196850106309</v>
       </c>
       <c r="F112" s="4">
@@ -3090,7 +3109,7 @@
       <c r="D113" s="4">
         <v>2819</v>
       </c>
-      <c r="E113" s="4">
+      <c r="E113" s="8">
         <v>8511778103071</v>
       </c>
       <c r="F113" s="4">

</xml_diff>